<commit_message>
Update Time Sheet Template 2024 v2 - 3.xlsx
</commit_message>
<xml_diff>
--- a/Personal/Others/Time Sheet Template 2024 v2 - 3.xlsx
+++ b/Personal/Others/Time Sheet Template 2024 v2 - 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asaklayen\Documents\App\MyAppData\Personal\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEE6951-10B2-4EFF-8E51-3A5F11D0A3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABF554-1668-436E-9F84-272D211CDEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="162">
   <si>
     <t xml:space="preserve">January </t>
   </si>
@@ -10534,7 +10534,7 @@
   <dimension ref="A1:AR148"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11066,13 +11066,25 @@
         <v>159</v>
       </c>
       <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="39"/>
+      <c r="G16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="K16" s="4">
         <v>3</v>
       </c>
@@ -11155,13 +11167,25 @@
         <v>120</v>
       </c>
       <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="39"/>
+      <c r="G17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>48</v>
+      </c>
       <c r="K17" s="4">
         <v>4</v>
       </c>
@@ -11591,7 +11615,7 @@
           <x14:formula1>
             <xm:f>'Data validation table'!$L$3:$L$54</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:H17</xm:sqref>
+          <xm:sqref>H15:H17 I16:J17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Engagement Function" prompt="Use the dropdown list" xr:uid="{8E05E90C-6CDC-4E63-8B53-488BCD4022C8}">
           <x14:formula1>

</xml_diff>